<commit_message>
edie code config mail
</commit_message>
<xml_diff>
--- a/uploads/imports/ยาง.xlsx
+++ b/uploads/imports/ยาง.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71329D1C-6847-4FF6-B53D-E6E99A82194B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{026EC31C-2FB8-43F6-8302-7B4ABCF391B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1845" yWindow="1890" windowWidth="21105" windowHeight="15135" xr2:uid="{F7D3303F-601B-4FF5-BD57-7CD5BA0A1BE7}"/>
+    <workbookView xWindow="8235" yWindow="3390" windowWidth="23580" windowHeight="17490" xr2:uid="{F7D3303F-601B-4FF5-BD57-7CD5BA0A1BE7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -477,7 +477,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="B13" sqref="B13:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -516,7 +516,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>2100000066</v>
+        <v>2100000073</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>9</v>
@@ -545,7 +545,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>2100000066</v>
+        <v>2100000073</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>9</v>
@@ -574,7 +574,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <v>2100000066</v>
+        <v>2100000073</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>9</v>
@@ -603,7 +603,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <v>2100000066</v>
+        <v>2100000073</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>9</v>
@@ -632,7 +632,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>2100000066</v>
+        <v>2100000073</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>9</v>
@@ -661,7 +661,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>2100000066</v>
+        <v>2100000073</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>9</v>
@@ -690,7 +690,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>2100000066</v>
+        <v>2100000073</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>9</v>
@@ -719,7 +719,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <v>2100000066</v>
+        <v>2100000073</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>9</v>

</xml_diff>